<commit_message>
vault backup: 2024-04-02 09:22:13
</commit_message>
<xml_diff>
--- a/projects/quote-process-optimization/cwsell-locations-matrix.xlsx
+++ b/projects/quote-process-optimization/cwsell-locations-matrix.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://meriplex-my.sharepoint.com/personal/ian_wheeler_meriplex_com/Documents/Documents/Obsidian/Meriplex/projects/quote-process-optimization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="38" documentId="8_{637A54EE-5991-4AE0-ABC0-C72358F341C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D2374350-55CC-4D0E-813C-01F105CFC1F0}"/>
+  <xr:revisionPtr revIDLastSave="39" documentId="8_{637A54EE-5991-4AE0-ABC0-C72358F341C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FA1A048D-4C00-4770-80A4-9E994EC32AB8}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="12852" windowWidth="23256" windowHeight="13896" xr2:uid="{4FE25E79-C121-4DA1-A7D4-492D09E1A43C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4FE25E79-C121-4DA1-A7D4-492D09E1A43C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Locations Matrix" sheetId="2" r:id="rId1"/>
-    <sheet name="Location Field Descriptions" sheetId="1" r:id="rId2"/>
+    <sheet name="Location Field Descriptions" sheetId="1" r:id="rId1"/>
+    <sheet name="Locations Matrix" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -259,18 +259,13 @@
   </cellStyles>
   <dxfs count="5">
     <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Display"/>
-        <family val="2"/>
-        <scheme val="major"/>
-      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -289,13 +284,18 @@
       <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Display"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -311,7 +311,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EAC0056F-81ED-46B4-9A13-395C0C8367F0}" name="Table2" displayName="Table2" ref="A1:R4" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{11AAA06B-52E6-451A-96B4-22CFEA1B6080}" name="Table1" displayName="Table1" ref="A1:B23" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
+  <autoFilter ref="A1:B23" xr:uid="{11AAA06B-52E6-451A-96B4-22CFEA1B6080}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{F13122CC-2313-40C2-A261-E09992C9FC9E}" name="Field" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{DE56D329-F22A-4EE7-982D-F1977A127CEF}" name="Description" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium22" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EAC0056F-81ED-46B4-9A13-395C0C8367F0}" name="Table2" displayName="Table2" ref="A1:R4" totalsRowShown="0" headerRowDxfId="4">
   <autoFilter ref="A1:R4" xr:uid="{EAC0056F-81ED-46B4-9A13-395C0C8367F0}"/>
   <tableColumns count="18">
     <tableColumn id="1" xr3:uid="{B7BBB3DC-B9C4-4295-B1A6-B21F3F0B422A}" name="Location Name"/>
@@ -332,17 +343,6 @@
     <tableColumn id="16" xr3:uid="{1B99D0D8-0E66-421D-9B7C-1D75739CC5D3}" name="Website"/>
     <tableColumn id="17" xr3:uid="{443D3D7B-5411-4309-AB80-8DDB72C46251}" name="Quote Prefix"/>
     <tableColumn id="18" xr3:uid="{9EC087A0-60E5-4B50-8A72-7F7D7E32AE66}" name="Quote Suffix"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium22" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{11AAA06B-52E6-451A-96B4-22CFEA1B6080}" name="Table1" displayName="Table1" ref="A1:B23" totalsRowShown="0" headerRowDxfId="1" dataDxfId="2">
-  <autoFilter ref="A1:B23" xr:uid="{11AAA06B-52E6-451A-96B4-22CFEA1B6080}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{F13122CC-2313-40C2-A261-E09992C9FC9E}" name="Field" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{DE56D329-F22A-4EE7-982D-F1977A127CEF}" name="Description" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium22" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -664,111 +664,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B252B40-5148-4FDB-83EF-710233DB49AD}">
-  <dimension ref="A1:R4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="18" width="30.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33D24721-5837-4A60-A669-863CE8326A23}">
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -968,4 +867,105 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B252B40-5148-4FDB-83EF-710233DB49AD}">
+  <dimension ref="A1:R4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="18" width="30.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>